<commit_message>
Tried to calculate the correct values for DAC and ADC setup, and created an interrupt routine to test them.  Calculator updated with relevant calculations
</commit_message>
<xml_diff>
--- a/Documentation/Calculators.xlsx
+++ b/Documentation/Calculators.xlsx
@@ -80,12 +80,11 @@
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>Fcy</t>
   </si>
@@ -151,6 +150,75 @@
   </si>
   <si>
     <t xml:space="preserve">*Used Excel solver to arrive at the numbers above </t>
+  </si>
+  <si>
+    <t>Desired Sample Rate</t>
+  </si>
+  <si>
+    <t>Required Clock Rate</t>
+  </si>
+  <si>
+    <t>Desired DACFDIV</t>
+  </si>
+  <si>
+    <t>Rounded DACFDIV</t>
+  </si>
+  <si>
+    <t>Actual Clock Rate</t>
+  </si>
+  <si>
+    <t>Actual Sample Rate</t>
+  </si>
+  <si>
+    <t>kHZ</t>
+  </si>
+  <si>
+    <t>DAC Clock</t>
+  </si>
+  <si>
+    <t>ADC Clock</t>
+  </si>
+  <si>
+    <t>TAD (min)</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>TAD</t>
+  </si>
+  <si>
+    <t>Tsamp (min)</t>
+  </si>
+  <si>
+    <t>Tcy</t>
+  </si>
+  <si>
+    <t>TAD (actual)</t>
+  </si>
+  <si>
+    <t>Tconv (typ)</t>
+  </si>
+  <si>
+    <t>ADCS (min)</t>
+  </si>
+  <si>
+    <t>ADCS (actual)</t>
+  </si>
+  <si>
+    <t>Tsamp (actual)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAD </t>
+  </si>
+  <si>
+    <t>Sample Rate (typ)</t>
+  </si>
+  <si>
+    <t>Period (typ)</t>
+  </si>
+  <si>
+    <t>kHz</t>
   </si>
 </sst>
 </file>
@@ -190,7 +258,7 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,8 +277,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -343,6 +417,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -355,7 +466,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -374,6 +485,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -396,16 +521,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>51736</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -429,13 +554,18 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5934075" y="314325"/>
-          <a:ext cx="7877175" cy="5505450"/>
+          <a:off x="6629400" y="380999"/>
+          <a:ext cx="6724650" cy="4699937"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
@@ -447,6 +577,160 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>164597</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6610351" y="5257800"/>
+          <a:ext cx="8089396" cy="6886575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5610225" y="381000"/>
+          <a:ext cx="1009650" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5619750" y="5038725"/>
+          <a:ext cx="962025" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -899,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F19"/>
+  <dimension ref="B4:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -917,6 +1201,9 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="2:6">
@@ -1015,31 +1302,280 @@
       <c r="E11" s="11"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" ht="15" thickBot="1">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="2:6" ht="15" thickBot="1">
-      <c r="B13" s="15" t="s">
+    <row r="13" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="31">
         <f>C11/2</f>
         <v>40</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B14" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="30">
+        <f>1/(C13/1000)</f>
+        <v>25</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="7">
+        <v>44.1</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="10"/>
+      <c r="C18" s="13">
+        <f>C17/1000</f>
+        <v>4.41E-2</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="13">
+        <f>C18*256</f>
+        <v>11.2896</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="13">
+        <f>C11/C19</f>
+        <v>7.0861678004535147</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="13">
+        <f>ROUND(C20, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="13">
+        <f>C11/C21</f>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="2:6" ht="15" thickBot="1">
+      <c r="B23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="26">
+        <f>C22/256</f>
+        <v>4.4642857142857144E-2</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B24" s="15"/>
+      <c r="C24" s="30">
+        <f>C23*1000</f>
+        <v>44.642857142857146</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="20">
+        <v>117.6</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="13">
+        <v>3</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="5">
+        <v>4</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="13">
+        <f>C14</f>
+        <v>25</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="13">
+        <f>C28/C31</f>
+        <v>4.7039999999999997</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="5">
+        <v>5</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="13">
+        <f>C33*C14</f>
+        <v>125</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="13">
+        <v>14</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="2:6" ht="15" thickBot="1">
+      <c r="B36" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="29">
+        <f>(C35+C30)*C34</f>
+        <v>2250</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B37" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="31">
+        <f>1/(C36*10^-6)</f>
+        <v>444.44444444444446</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="24"/>
+      <c r="F37" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More code modularization, added the Family Reference document for the TIMER module
</commit_message>
<xml_diff>
--- a/Documentation/Calculators.xlsx
+++ b/Documentation/Calculators.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>Fcy</t>
   </si>
@@ -176,9 +176,6 @@
     <t>DAC Clock</t>
   </si>
   <si>
-    <t>ADC Clock</t>
-  </si>
-  <si>
     <t>TAD (min)</t>
   </si>
   <si>
@@ -219,6 +216,12 @@
   </si>
   <si>
     <t>kHz</t>
+  </si>
+  <si>
+    <t>ADC Clock (deriving from system)</t>
+  </si>
+  <si>
+    <t>ADC Clock (deriving from RC_ADC)</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>51736</xdr:rowOff>
+      <xdr:rowOff>42211</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -590,7 +593,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>164597</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -731,6 +734,126 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>665389</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>156482</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13364936" y="372836"/>
+          <a:ext cx="3125560" cy="4015467"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12246</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>63953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16572138" y="366032"/>
+          <a:ext cx="6755947" cy="3371850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1183,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F37"/>
+  <dimension ref="B4:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1325,14 +1448,14 @@
     </row>
     <row r="14" spans="2:6" ht="15.75" thickBot="1">
       <c r="B14" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="30">
         <f>1/(C13/1000)</f>
         <v>25</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="17"/>
@@ -1386,20 +1509,20 @@
         <v>24</v>
       </c>
       <c r="C20" s="13">
-        <f>C11/C19</f>
-        <v>7.0861678004535147</v>
+        <f>C9/C19</f>
+        <v>14.172335600907029</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" ht="15">
       <c r="B21" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="13">
-        <f>ROUND(C20, 0)</f>
-        <v>7</v>
+      <c r="C21" s="14">
+        <f>ROUNDUP(C20, 0)</f>
+        <v>15</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
@@ -1410,8 +1533,8 @@
         <v>26</v>
       </c>
       <c r="C22" s="13">
-        <f>C11/C21</f>
-        <v>11.428571428571429</v>
+        <f>C9/C21</f>
+        <v>10.666666666666666</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
@@ -1423,7 +1546,7 @@
       </c>
       <c r="C23" s="26">
         <f>C22/256</f>
-        <v>4.4642857142857144E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1433,7 +1556,7 @@
       <c r="B24" s="15"/>
       <c r="C24" s="30">
         <f>C23*1000</f>
-        <v>44.642857142857146</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>28</v>
@@ -1443,65 +1566,65 @@
     </row>
     <row r="27" spans="2:6" ht="15.75" thickBot="1">
       <c r="B27" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="20">
         <v>117.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="13">
         <v>3</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="12"/>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="C30" s="5">
-        <v>4</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="12"/>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="13">
         <f>C14</f>
         <v>25</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="12"/>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="13">
         <f>C28/C31</f>
@@ -1513,10 +1636,10 @@
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="5">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
@@ -1524,62 +1647,200 @@
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="13">
         <f>C33*C14</f>
-        <v>125</v>
+        <v>1250</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="12"/>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="13">
         <v>14</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="2:6" ht="15" thickBot="1">
       <c r="B36" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" s="29">
         <f>(C35+C30)*C34</f>
-        <v>2250</v>
+        <v>23750</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="12"/>
     </row>
     <row r="37" spans="2:6" ht="15.75" thickBot="1">
       <c r="B37" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" s="31">
         <f>1/(C36*10^-6)</f>
-        <v>444.44444444444446</v>
+        <v>42.10526315789474</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="25"/>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B41" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="20">
+        <v>117.6</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="13">
+        <v>3</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="5">
+        <v>5</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="13">
+        <v>250</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="13">
+        <f>C42/C45</f>
+        <v>0.47039999999999998</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="5">
+        <v>5</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="13">
+        <f>C47*C45</f>
+        <v>1250</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="12"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="13">
+        <v>14</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="11"/>
+      <c r="F49" s="12"/>
+    </row>
+    <row r="50" spans="2:6" ht="15" thickBot="1">
+      <c r="B50" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="29">
+        <f>(C49+C44)*C48</f>
+        <v>23750</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="11"/>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B51" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="31">
+        <f>1/(C50*10^-6)</f>
+        <v>42.10526315789474</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="24"/>
+      <c r="F51" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C21" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added UART code, added the UART family reference guide.  Created interrupt routines for the UART.
</commit_message>
<xml_diff>
--- a/Documentation/Calculators.xlsx
+++ b/Documentation/Calculators.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>Fcy</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>ADC Clock (deriving from RC_ADC)</t>
+  </si>
+  <si>
+    <t>UART BAUD</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>164597</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>24493</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -854,6 +857,113 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>312964</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>176892</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>42181</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>48985</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6613071" y="12178392"/>
+          <a:ext cx="7213146" cy="7492093"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>258536</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5646964" y="11293929"/>
+          <a:ext cx="911679" cy="966107"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1306,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F51"/>
+  <dimension ref="B4:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1834,6 +1944,81 @@
       </c>
       <c r="E51" s="24"/>
       <c r="F51" s="25"/>
+    </row>
+    <row r="62" spans="2:6" ht="15" thickBot="1">
+      <c r="B62" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" s="6"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="10"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="10"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="12"/>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" s="10"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="10"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="12"/>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="10"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="12"/>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" s="10"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="12"/>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="10"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="12"/>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="10"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="12"/>
+    </row>
+    <row r="72" spans="2:6" ht="15" thickBot="1">
+      <c r="B72" s="15"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added some highlights to the datasheet and added some calculations.  These need to be cleaned up
</commit_message>
<xml_diff>
--- a/Documentation/Calculators.xlsx
+++ b/Documentation/Calculators.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Unknown" sheetId="1" r:id="rId1"/>
     <sheet name="Clocks" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sampling and Storage" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Clocks!$C$6,Clocks!$C$8,Clocks!$C$10</definedName>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
   <si>
     <t>Fcy</t>
   </si>
@@ -225,6 +225,36 @@
   </si>
   <si>
     <t>UART BAUD</t>
+  </si>
+  <si>
+    <t>Fadc</t>
+  </si>
+  <si>
+    <t>Fdac</t>
+  </si>
+  <si>
+    <t>Tadc</t>
+  </si>
+  <si>
+    <t>Tdac</t>
+  </si>
+  <si>
+    <t>nS</t>
+  </si>
+  <si>
+    <t>mS</t>
+  </si>
+  <si>
+    <t>Fmod</t>
+  </si>
+  <si>
+    <t>Tmod</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>Samples per period @ DAC rate</t>
   </si>
 </sst>
 </file>
@@ -472,7 +502,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -505,6 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -1418,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2032,12 +2063,113 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="32">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="32">
+        <f>1/(C3*1)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="32">
+        <f>Clocks!C37</f>
+        <v>42.10526315789474</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="32">
+        <f>1/(C4/1000)</f>
+        <v>23.749999999999996</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="32">
+        <f>Clocks!C24</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="32">
+        <f>1/(C5/1000)</f>
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>500</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8">
+        <f>1/(C8/1000)</f>
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15">
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="3">
+        <f>(F8*1000)/F5</f>
+        <v>83.333333333333329</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>